<commit_message>
move past merge conflict.  repoint directories
</commit_message>
<xml_diff>
--- a/Export/Securities_DD_wRemaining.xlsx
+++ b/Export/Securities_DD_wRemaining.xlsx
@@ -1,26 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24931"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/cdc4f9836624c718/Documents/Grad-School-Docs/CapstoneProject/Repo/Export/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="11_2D6674DBC91565DEF0170B83FB2D42615E2AE6A9" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{96E7DE2E-5929-4CAF-95B0-B3F6E0B4E5E7}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-105" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Securities_Remaining" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="113">
   <si>
     <t>Mnemonic</t>
   </si>
@@ -359,49 +353,13 @@
   </si>
   <si>
     <t>State/Province</t>
-  </si>
-  <si>
-    <t>Tier</t>
-  </si>
-  <si>
-    <t>Note</t>
-  </si>
-  <si>
-    <t>1- Absolutely Keep</t>
-  </si>
-  <si>
-    <t>2- Likey Keep</t>
-  </si>
-  <si>
-    <t>3- Likely Delete</t>
-  </si>
-  <si>
-    <t>4- Absolutely Delete</t>
-  </si>
-  <si>
-    <t>5x- Combo Candidate</t>
-  </si>
-  <si>
-    <t>6x-Will Combine</t>
-  </si>
-  <si>
-    <t>No need for this</t>
-  </si>
-  <si>
-    <t>A- Level</t>
-  </si>
-  <si>
-    <t>Most likely from Stocks Dataset -- come back if not</t>
-  </si>
-  <si>
-    <t>A+ Level</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -426,7 +384,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -449,25 +407,13 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -476,14 +422,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -530,7 +468,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -562,27 +500,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -614,24 +534,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -807,19 +709,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M56"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="8" max="8" width="17.44140625" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -829,32 +726,8 @@
       <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="H1" t="s">
-        <v>115</v>
-      </c>
-      <c r="I1" t="s">
-        <v>116</v>
-      </c>
-      <c r="J1" t="s">
-        <v>117</v>
-      </c>
-      <c r="K1" t="s">
-        <v>118</v>
-      </c>
-      <c r="L1" t="s">
-        <v>119</v>
-      </c>
-      <c r="M1" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -868,7 +741,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -881,14 +754,8 @@
       <c r="D3">
         <v>0</v>
       </c>
-      <c r="E3">
-        <v>4</v>
-      </c>
-      <c r="F3" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="1:4">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -902,7 +769,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -915,14 +782,8 @@
       <c r="D5">
         <v>0</v>
       </c>
-      <c r="E5">
-        <v>4</v>
-      </c>
-      <c r="F5" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="6" spans="1:4">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -936,7 +797,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -949,14 +810,8 @@
       <c r="D7">
         <v>1</v>
       </c>
-      <c r="E7">
-        <v>1</v>
-      </c>
-      <c r="F7" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="8" spans="1:4">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -969,14 +824,8 @@
       <c r="D8">
         <v>1</v>
       </c>
-      <c r="E8">
-        <v>1</v>
-      </c>
-      <c r="F8" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="9" spans="1:4">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -990,7 +839,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -1004,7 +853,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -1018,7 +867,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -1032,7 +881,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -1046,7 +895,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -1060,7 +909,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -1074,7 +923,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -1088,7 +937,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4">
       <c r="A17" s="1">
         <v>15</v>
       </c>
@@ -1102,7 +951,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4">
       <c r="A18" s="1">
         <v>16</v>
       </c>
@@ -1116,7 +965,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4">
       <c r="A19" s="1">
         <v>17</v>
       </c>
@@ -1130,7 +979,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4">
       <c r="A20" s="1">
         <v>18</v>
       </c>
@@ -1143,14 +992,8 @@
       <c r="D20">
         <v>0</v>
       </c>
-      <c r="E20">
-        <v>4</v>
-      </c>
-      <c r="F20" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="21" spans="1:4">
       <c r="A21" s="1">
         <v>19</v>
       </c>
@@ -1164,7 +1007,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4">
       <c r="A22" s="1">
         <v>20</v>
       </c>
@@ -1178,7 +1021,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4">
       <c r="A23" s="1">
         <v>21</v>
       </c>
@@ -1191,14 +1034,8 @@
       <c r="D23">
         <v>0</v>
       </c>
-      <c r="E23">
-        <v>4</v>
-      </c>
-      <c r="F23" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="24" spans="1:4">
       <c r="A24" s="1">
         <v>22</v>
       </c>
@@ -1211,14 +1048,8 @@
       <c r="D24">
         <v>0</v>
       </c>
-      <c r="E24">
-        <v>4</v>
-      </c>
-      <c r="F24" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="25" spans="1:4">
       <c r="A25" s="1">
         <v>23</v>
       </c>
@@ -1231,14 +1062,8 @@
       <c r="D25">
         <v>0</v>
       </c>
-      <c r="E25">
-        <v>4</v>
-      </c>
-      <c r="F25" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="26" spans="1:4">
       <c r="A26" s="1">
         <v>24</v>
       </c>
@@ -1251,14 +1076,8 @@
       <c r="D26">
         <v>0</v>
       </c>
-      <c r="E26">
-        <v>1</v>
-      </c>
-      <c r="F26" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="27" spans="1:4">
       <c r="A27" s="1">
         <v>25</v>
       </c>
@@ -1271,14 +1090,8 @@
       <c r="D27">
         <v>0</v>
       </c>
-      <c r="E27">
-        <v>1</v>
-      </c>
-      <c r="F27" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="28" spans="1:4">
       <c r="A28" s="1">
         <v>26</v>
       </c>
@@ -1292,7 +1105,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4">
       <c r="A29" s="1">
         <v>27</v>
       </c>
@@ -1306,7 +1119,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4">
       <c r="A30" s="1">
         <v>28</v>
       </c>
@@ -1320,7 +1133,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4">
       <c r="A31" s="1">
         <v>29</v>
       </c>
@@ -1334,7 +1147,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4">
       <c r="A32" s="1">
         <v>30</v>
       </c>
@@ -1348,7 +1161,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4">
       <c r="A33" s="1">
         <v>31</v>
       </c>
@@ -1362,7 +1175,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4">
       <c r="A34" s="1">
         <v>32</v>
       </c>
@@ -1376,7 +1189,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4">
       <c r="A35" s="1">
         <v>33</v>
       </c>
@@ -1390,7 +1203,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4">
       <c r="A36" s="1">
         <v>34</v>
       </c>
@@ -1404,7 +1217,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4">
       <c r="A37" s="1">
         <v>35</v>
       </c>
@@ -1418,7 +1231,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4">
       <c r="A38" s="1">
         <v>36</v>
       </c>
@@ -1432,7 +1245,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4">
       <c r="A39" s="1">
         <v>37</v>
       </c>
@@ -1446,7 +1259,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:4">
       <c r="A40" s="1">
         <v>38</v>
       </c>
@@ -1459,14 +1272,8 @@
       <c r="D40">
         <v>0</v>
       </c>
-      <c r="E40">
-        <v>4</v>
-      </c>
-      <c r="F40" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="41" spans="1:4">
       <c r="A41" s="1">
         <v>39</v>
       </c>
@@ -1479,14 +1286,8 @@
       <c r="D41">
         <v>0</v>
       </c>
-      <c r="E41">
-        <v>4</v>
-      </c>
-      <c r="F41" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="42" spans="1:4">
       <c r="A42" s="1">
         <v>40</v>
       </c>
@@ -1500,7 +1301,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:4">
       <c r="A43" s="1">
         <v>41</v>
       </c>
@@ -1514,7 +1315,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:4">
       <c r="A44" s="1">
         <v>42</v>
       </c>
@@ -1527,14 +1328,8 @@
       <c r="D44">
         <v>0</v>
       </c>
-      <c r="E44">
-        <v>4</v>
-      </c>
-      <c r="F44" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="45" spans="1:4">
       <c r="A45" s="1">
         <v>43</v>
       </c>
@@ -1547,14 +1342,8 @@
       <c r="D45">
         <v>0</v>
       </c>
-      <c r="E45">
-        <v>4</v>
-      </c>
-      <c r="F45" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="46" spans="1:4">
       <c r="A46" s="1">
         <v>44</v>
       </c>
@@ -1568,7 +1357,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:4">
       <c r="A47" s="1">
         <v>45</v>
       </c>
@@ -1582,7 +1371,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:4">
       <c r="A48" s="1">
         <v>46</v>
       </c>
@@ -1596,7 +1385,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:4">
       <c r="A49" s="1">
         <v>47</v>
       </c>
@@ -1610,7 +1399,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:4">
       <c r="A50" s="1">
         <v>48</v>
       </c>
@@ -1624,7 +1413,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:4">
       <c r="A51" s="1">
         <v>49</v>
       </c>
@@ -1638,7 +1427,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:4">
       <c r="A52" s="1">
         <v>50</v>
       </c>
@@ -1652,7 +1441,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:4">
       <c r="A53" s="1">
         <v>51</v>
       </c>
@@ -1666,7 +1455,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:4">
       <c r="A54" s="1">
         <v>52</v>
       </c>
@@ -1680,7 +1469,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:4">
       <c r="A55" s="1">
         <v>53</v>
       </c>
@@ -1694,7 +1483,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:4">
       <c r="A56" s="1">
         <v>54</v>
       </c>

</xml_diff>